<commit_message>
un es1 fatto + scaricate soluzioni
</commit_message>
<xml_diff>
--- a/Esercitazioni_AC/2022_02_14/Nome_Cognome_Es1_CEM_14_02_2022.xlsx
+++ b/Esercitazioni_AC/2022_02_14/Nome_Cognome_Es1_CEM_14_02_2022.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="131">
   <si>
     <r>
       <rPr>
@@ -305,37 +305,27 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Tempo minimo di esecuzione = 15</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.      Si disegni il grafo delle dipendenze e si deduca il numero minimo di periodi di clock necessario a eseguire il codice assegnato tenendo conto solo delle dipendenze trovate (1 punto).</t>
   </si>
   <si>
     <t xml:space="preserve">Alee: (WAW, RAW, WAR) #si inseriscano le alee presenti per istruzione.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Da completare con la soluzione dell'esercizio.  Si riporti il grafo delle dipendenze e si deduca il numero minimo di periodi di clock necessario a eseguire il codice assegnato tenendo conto solo delle dipendenze trovate.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">RAW f1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAW f5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAW f5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Da completare con la soluzione dell'esercizio.  Si riporti il grafo delle dipendenze e si deduca il numero minimo di periodi di clock necessario a eseguire il codice assegnato tenendo conto solo delle dipendenze trovate.
 Si codifichi il grafo delle dipendenze come una lista con il seguente formato:
 si descrivano i nodi del grafo tra parentesi tonde. Separando il numero dell'istruzione ed il numero di cicli spesi in execute dell'istruzione con una virgola all'interno di parentesi tonde. Es.: (id_istruzione, numero_cicli) </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Dipendenze</t>
@@ -357,6 +347,21 @@
   </si>
   <si>
     <t xml:space="preserve">Tot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,2)→(2,3)→</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,4)-&gt;(5,3)-&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,4)→(6,4)→</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,2)→(4,4)→</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempo minimo di esecuzione = 12</t>
   </si>
   <si>
     <t xml:space="preserve">3.      Si mostri la dinamica dell’esecuzione nel caso della CPU considerata nel punto 1 con 1 CRB, uno stadio di IF e uno di ID, e 2 RS per ognuna delle tre unità funzionali </t>
@@ -506,22 +511,55 @@
     <t xml:space="preserve">f3</t>
   </si>
   <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A0_E</t>
+  </si>
+  <si>
     <t xml:space="preserve">f5</t>
   </si>
   <si>
     <t xml:space="preserve">f4</t>
   </si>
   <si>
+    <t xml:space="preserve">IF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MO_W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MO_E</t>
+  </si>
+  <si>
     <t xml:space="preserve">f16</t>
   </si>
   <si>
     <t xml:space="preserve">f8</t>
   </si>
   <si>
+    <t xml:space="preserve">D0_E</t>
+  </si>
+  <si>
     <t xml:space="preserve">f6</t>
   </si>
   <si>
+    <t xml:space="preserve">D1_R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_E</t>
+  </si>
+  <si>
     <t xml:space="preserve">f7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1_W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1_E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D0_R</t>
   </si>
   <si>
     <t xml:space="preserve">4.      E’ possibile ridurre il numero di periodi di clock necessario ad eseguire il codice assegnato rispetto al valore risultante dalla risposta al punto 3? Si punti al numero minore possibile di periodi di clock e al numero minimo di modifiche, supponendo di poter apportare solo le seguenti modifiche all’architettura: </t>
@@ -670,6 +708,12 @@
     <t xml:space="preserve"># numero CRB complessivo.</t>
   </si>
   <si>
+    <t xml:space="preserve">X0_E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_W</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -701,6 +745,12 @@
   <si>
     <t xml:space="preserve">Val</t>
   </si>
+  <si>
+    <t xml:space="preserve">MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO</t>
+  </si>
 </sst>
 </file>
 
@@ -709,7 +759,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -811,12 +861,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -858,6 +906,11 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -878,6 +931,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1151,7 +1211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1264,6 +1324,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1276,10 +1340,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1448,15 +1508,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1464,7 +1532,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1488,6 +1556,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1549,6 +1621,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1738,7 +1814,7 @@
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V22" activeCellId="0" sqref="V22"/>
+      <selection pane="topLeft" activeCell="Z23" activeCellId="0" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2162,16 +2238,24 @@
         <v>32</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
+      <c r="C17" s="19" t="n">
+        <v>1</v>
+      </c>
       <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
+      <c r="H17" s="20" t="n">
+        <v>3</v>
+      </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="L17" s="20" t="n">
+        <v>5</v>
+      </c>
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
@@ -2181,16 +2265,24 @@
         <v>33</v>
       </c>
       <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
+      <c r="C18" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="19" t="n">
+        <v>3</v>
+      </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
+      <c r="H18" s="20" t="n">
+        <v>3</v>
+      </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
+      <c r="L18" s="21" t="n">
+        <v>9</v>
+      </c>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
       <c r="O18" s="21"/>
@@ -2200,16 +2292,24 @@
         <v>34</v>
       </c>
       <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
+      <c r="C19" s="19" t="n">
+        <v>3</v>
+      </c>
       <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="19" t="n">
+        <v>4</v>
+      </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
+      <c r="H19" s="20" t="n">
+        <v>3</v>
+      </c>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
-      <c r="L19" s="22"/>
+      <c r="L19" s="22" t="n">
+        <v>15</v>
+      </c>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
@@ -2234,7 +2334,9 @@
       <c r="O21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23"/>
+      <c r="A22" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -2367,8 +2469,8 @@
   </sheetPr>
   <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q27" activeCellId="0" sqref="Q27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2391,7 +2493,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -2445,7 +2547,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -2523,7 +2625,9 @@
       <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
       <c r="G4" s="27" t="s">
@@ -2548,7 +2652,9 @@
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
       <c r="G5" s="27" t="s">
@@ -2573,7 +2679,9 @@
       <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
     </row>
@@ -2587,7 +2695,9 @@
       <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
     </row>
@@ -2601,9 +2711,11 @@
       <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="D8" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
@@ -2767,7 +2879,7 @@
     </row>
     <row r="15" customFormat="false" ht="127.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -2785,25 +2897,25 @@
       <c r="O15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
+      <c r="A16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
@@ -2835,115 +2947,163 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30" t="s">
+      <c r="E17" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="20"/>
+      <c r="A19" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="G19" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="I19" s="20" t="n">
+        <v>5</v>
+      </c>
       <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="K19" s="20" t="n">
+        <v>2</v>
+      </c>
       <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
+      <c r="M19" s="21" t="n">
+        <v>9</v>
+      </c>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="20"/>
+      <c r="A20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+      <c r="G20" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="I20" s="20" t="n">
+        <v>7</v>
+      </c>
       <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="K20" s="20" t="n">
+        <v>2</v>
+      </c>
       <c r="L20" s="20"/>
-      <c r="M20" s="21"/>
+      <c r="M20" s="21" t="n">
+        <v>11</v>
+      </c>
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="20"/>
+      <c r="A21" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="G21" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="n">
+        <v>8</v>
+      </c>
       <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="K21" s="20" t="n">
+        <v>2</v>
+      </c>
       <c r="L21" s="20"/>
-      <c r="M21" s="32"/>
+      <c r="M21" s="32" t="n">
+        <v>12</v>
+      </c>
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="20"/>
+      <c r="A22" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
+      <c r="G22" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="20" t="n">
+        <v>6</v>
+      </c>
       <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="20" t="n">
+        <v>2</v>
+      </c>
       <c r="L22" s="20"/>
-      <c r="M22" s="32"/>
+      <c r="M22" s="32" t="n">
+        <v>10</v>
+      </c>
       <c r="N22" s="32"/>
       <c r="O22" s="32"/>
     </row>
@@ -2981,7 +3141,9 @@
       <c r="Q24" s="33"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22"/>
+      <c r="A25" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -3313,7 +3475,7 @@
   <dimension ref="A1:AW19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="AQ20" activeCellId="0" sqref="AQ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3337,7 +3499,7 @@
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -3377,7 +3539,7 @@
       <c r="AK1" s="35"/>
       <c r="AL1" s="35"/>
       <c r="AM1" s="36" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="AN1" s="36"/>
       <c r="AO1" s="36"/>
@@ -3386,7 +3548,7 @@
     </row>
     <row r="2" s="40" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -3586,7 +3748,7 @@
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -3641,7 +3803,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="53" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="53"/>
@@ -3694,7 +3856,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="54" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B10" s="54"/>
       <c r="C10" s="54"/>
@@ -3750,245 +3912,245 @@
         <v>1</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G11" s="58"/>
       <c r="H11" s="57" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I11" s="58"/>
       <c r="J11" s="59" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="K11" s="58"/>
       <c r="L11" s="57" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="M11" s="58"/>
       <c r="N11" s="57" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="O11" s="58"/>
       <c r="P11" s="57" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="Q11" s="58"/>
       <c r="R11" s="57" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="S11" s="58"/>
       <c r="T11" s="57" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="U11" s="58"/>
       <c r="V11" s="57" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="W11" s="58"/>
       <c r="X11" s="59" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="Y11" s="58"/>
       <c r="Z11" s="57" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="AA11" s="58"/>
       <c r="AB11" s="57" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="AC11" s="58"/>
       <c r="AD11" s="57" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="AE11" s="58"/>
       <c r="AF11" s="57" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="AG11" s="58"/>
       <c r="AH11" s="57" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="AI11" s="58"/>
       <c r="AJ11" s="57" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="AK11" s="58"/>
       <c r="AL11" s="57" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="AM11" s="58"/>
       <c r="AN11" s="57" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="AO11" s="58"/>
       <c r="AP11" s="57" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="AQ11" s="58"/>
       <c r="AR11" s="57" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AS11" s="58"/>
       <c r="AT11" s="60" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AU11" s="60"/>
       <c r="AV11" s="60" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AW11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="61"/>
       <c r="B12" s="62" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
       <c r="F12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="J12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="L12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="M12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="N12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="O12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="P12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="Q12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="R12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="S12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="T12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="U12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="V12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="W12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="X12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="Y12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="Z12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AA12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AB12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AC12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AD12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AE12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AG12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AH12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AI12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AJ12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AK12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AL12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AM12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AN12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AO12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AP12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AQ12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AR12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AS12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AT12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AU12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AV12" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AW12" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,23 +4161,33 @@
         <v>4</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E13" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="67"/>
+        <v>92</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>46</v>
+      </c>
       <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
+      <c r="H13" s="67" t="s">
+        <v>93</v>
+      </c>
       <c r="I13" s="67"/>
-      <c r="J13" s="68"/>
+      <c r="J13" s="68" t="s">
+        <v>94</v>
+      </c>
       <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
+      <c r="L13" s="68" t="s">
+        <v>94</v>
+      </c>
       <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
+      <c r="N13" s="68" t="s">
+        <v>48</v>
+      </c>
       <c r="O13" s="68"/>
       <c r="P13" s="68"/>
       <c r="Q13" s="68"/>
@@ -4060,32 +4232,48 @@
         <v>7</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D14" s="71" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F14" s="73"/>
       <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
+      <c r="H14" s="73" t="s">
+        <v>97</v>
+      </c>
       <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
+      <c r="J14" s="73" t="s">
+        <v>93</v>
+      </c>
       <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
+      <c r="L14" s="73" t="s">
+        <v>98</v>
+      </c>
       <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
+      <c r="N14" s="73" t="s">
+        <v>98</v>
+      </c>
       <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
+      <c r="P14" s="73" t="s">
+        <v>99</v>
+      </c>
       <c r="Q14" s="73"/>
-      <c r="R14" s="73"/>
-      <c r="S14" s="73"/>
-      <c r="T14" s="73"/>
-      <c r="U14" s="73"/>
-      <c r="V14" s="73"/>
-      <c r="W14" s="73"/>
+      <c r="R14" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="S14" s="74"/>
+      <c r="T14" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="W14" s="74"/>
       <c r="X14" s="68"/>
       <c r="Y14" s="68"/>
       <c r="Z14" s="68"/>
@@ -4121,33 +4309,49 @@
         <v>10</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="74" t="s">
-        <v>87</v>
+        <v>100</v>
+      </c>
+      <c r="E15" s="75" t="s">
+        <v>101</v>
       </c>
       <c r="F15" s="73"/>
       <c r="G15" s="73"/>
       <c r="H15" s="73"/>
       <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
+      <c r="J15" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
+      <c r="L15" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
+      <c r="N15" s="73" t="s">
+        <v>102</v>
+      </c>
       <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="73"/>
-      <c r="V15" s="73"/>
+      <c r="P15" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="S15" s="74"/>
+      <c r="T15" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="U15" s="74"/>
+      <c r="V15" s="73" t="s">
+        <v>48</v>
+      </c>
       <c r="W15" s="73"/>
-      <c r="X15" s="73"/>
+      <c r="X15" s="73" t="s">
+        <v>48</v>
+      </c>
       <c r="Y15" s="73"/>
       <c r="Z15" s="68"/>
       <c r="AA15" s="68"/>
@@ -4182,13 +4386,13 @@
         <v>10</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="F16" s="73"/>
       <c r="G16" s="73"/>
@@ -4196,25 +4400,45 @@
       <c r="I16" s="73"/>
       <c r="J16" s="73"/>
       <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
+      <c r="L16" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
+      <c r="N16" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="68"/>
-      <c r="Y16" s="68"/>
-      <c r="Z16" s="68"/>
-      <c r="AA16" s="68"/>
-      <c r="AB16" s="68"/>
-      <c r="AC16" s="68"/>
-      <c r="AD16" s="68"/>
+      <c r="P16" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q16" s="68"/>
+      <c r="R16" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="S16" s="76"/>
+      <c r="T16" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="U16" s="76"/>
+      <c r="V16" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="W16" s="68"/>
+      <c r="X16" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA16" s="76"/>
+      <c r="AB16" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC16" s="76"/>
+      <c r="AD16" s="68" t="s">
+        <v>48</v>
+      </c>
       <c r="AE16" s="68"/>
       <c r="AF16" s="68"/>
       <c r="AG16" s="68"/>
@@ -4243,13 +4467,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E17" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="F17" s="73"/>
       <c r="G17" s="73"/>
@@ -4259,25 +4483,45 @@
       <c r="K17" s="73"/>
       <c r="L17" s="73"/>
       <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
+      <c r="N17" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="O17" s="73"/>
-      <c r="P17" s="73"/>
+      <c r="P17" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
-      <c r="S17" s="73"/>
-      <c r="T17" s="73"/>
-      <c r="U17" s="73"/>
-      <c r="V17" s="73"/>
-      <c r="W17" s="73"/>
-      <c r="X17" s="68"/>
-      <c r="Y17" s="68"/>
-      <c r="Z17" s="68"/>
-      <c r="AA17" s="68"/>
-      <c r="AB17" s="68"/>
-      <c r="AC17" s="68"/>
-      <c r="AD17" s="68"/>
-      <c r="AE17" s="68"/>
-      <c r="AF17" s="68"/>
+      <c r="R17" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="S17" s="74"/>
+      <c r="T17" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="U17" s="74"/>
+      <c r="V17" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="W17" s="74"/>
+      <c r="X17" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y17" s="76"/>
+      <c r="Z17" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA17" s="76"/>
+      <c r="AB17" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC17" s="76"/>
+      <c r="AD17" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE17" s="76"/>
+      <c r="AF17" s="68" t="s">
+        <v>48</v>
+      </c>
       <c r="AG17" s="68"/>
       <c r="AH17" s="68"/>
       <c r="AI17" s="68"/>
@@ -4304,13 +4548,13 @@
         <v>10</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D18" s="70" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E18" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
@@ -4322,34 +4566,60 @@
       <c r="M18" s="68"/>
       <c r="N18" s="68"/>
       <c r="O18" s="68"/>
-      <c r="P18" s="73"/>
+      <c r="P18" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="Q18" s="73"/>
-      <c r="R18" s="73"/>
+      <c r="R18" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="S18" s="73"/>
-      <c r="T18" s="73"/>
+      <c r="T18" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="U18" s="73"/>
-      <c r="V18" s="73"/>
+      <c r="V18" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="W18" s="73"/>
-      <c r="X18" s="73"/>
+      <c r="X18" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="Y18" s="73"/>
-      <c r="Z18" s="73"/>
-      <c r="AA18" s="73"/>
-      <c r="AB18" s="73"/>
+      <c r="Z18" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="74"/>
+      <c r="AB18" s="73" t="s">
+        <v>109</v>
+      </c>
       <c r="AC18" s="73"/>
-      <c r="AD18" s="73"/>
-      <c r="AE18" s="73"/>
-      <c r="AF18" s="68"/>
-      <c r="AG18" s="68"/>
-      <c r="AH18" s="73"/>
-      <c r="AI18" s="73"/>
-      <c r="AJ18" s="73"/>
-      <c r="AK18" s="73"/>
-      <c r="AL18" s="73"/>
-      <c r="AM18" s="73"/>
-      <c r="AN18" s="68"/>
-      <c r="AO18" s="68"/>
-      <c r="AP18" s="68"/>
-      <c r="AQ18" s="68"/>
+      <c r="AD18" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE18" s="74"/>
+      <c r="AF18" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG18" s="74"/>
+      <c r="AH18" s="76" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI18" s="76"/>
+      <c r="AJ18" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK18" s="74"/>
+      <c r="AL18" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM18" s="74"/>
+      <c r="AN18" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO18" s="73"/>
+      <c r="AP18" s="73"/>
+      <c r="AQ18" s="73"/>
       <c r="AR18" s="68"/>
       <c r="AS18" s="68"/>
       <c r="AT18" s="68"/>
@@ -4536,8 +4806,8 @@
   </sheetPr>
   <dimension ref="A1:AW29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF12" activeCellId="0" sqref="AF12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4560,305 +4830,305 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="75" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="75"/>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="75"/>
+      <c r="A1" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="77"/>
+      <c r="AT1" s="77"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="Z2" s="76"/>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="76"/>
-      <c r="AC2" s="76"/>
-      <c r="AD2" s="76"/>
-      <c r="AE2" s="76"/>
-      <c r="AF2" s="76"/>
-      <c r="AG2" s="76"/>
-      <c r="AH2" s="76"/>
-      <c r="AI2" s="76"/>
-      <c r="AJ2" s="76"/>
-      <c r="AK2" s="76"/>
-      <c r="AL2" s="76"/>
-      <c r="AM2" s="76"/>
-      <c r="AN2" s="76"/>
-      <c r="AO2" s="76"/>
-      <c r="AP2" s="76"/>
-      <c r="AQ2" s="76"/>
-      <c r="AR2" s="76"/>
-      <c r="AS2" s="76"/>
-      <c r="AT2" s="76"/>
+      <c r="A2" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="78"/>
+      <c r="AK2" s="78"/>
+      <c r="AL2" s="78"/>
+      <c r="AM2" s="78"/>
+      <c r="AN2" s="78"/>
+      <c r="AO2" s="78"/>
+      <c r="AP2" s="78"/>
+      <c r="AQ2" s="78"/>
+      <c r="AR2" s="78"/>
+      <c r="AS2" s="78"/>
+      <c r="AT2" s="78"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="76"/>
-      <c r="AC3" s="76"/>
-      <c r="AD3" s="76"/>
-      <c r="AE3" s="76"/>
-      <c r="AF3" s="76"/>
-      <c r="AG3" s="76"/>
-      <c r="AH3" s="76"/>
-      <c r="AI3" s="76"/>
-      <c r="AJ3" s="76"/>
-      <c r="AK3" s="76"/>
-      <c r="AL3" s="76"/>
-      <c r="AM3" s="76"/>
-      <c r="AN3" s="76"/>
-      <c r="AO3" s="76"/>
-      <c r="AP3" s="76"/>
-      <c r="AQ3" s="76"/>
-      <c r="AR3" s="76"/>
-      <c r="AS3" s="76"/>
-      <c r="AT3" s="76"/>
+      <c r="A3" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="78"/>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="78"/>
+      <c r="AD3" s="78"/>
+      <c r="AE3" s="78"/>
+      <c r="AF3" s="78"/>
+      <c r="AG3" s="78"/>
+      <c r="AH3" s="78"/>
+      <c r="AI3" s="78"/>
+      <c r="AJ3" s="78"/>
+      <c r="AK3" s="78"/>
+      <c r="AL3" s="78"/>
+      <c r="AM3" s="78"/>
+      <c r="AN3" s="78"/>
+      <c r="AO3" s="78"/>
+      <c r="AP3" s="78"/>
+      <c r="AQ3" s="78"/>
+      <c r="AR3" s="78"/>
+      <c r="AS3" s="78"/>
+      <c r="AT3" s="78"/>
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="76"/>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="76"/>
-      <c r="AE4" s="76"/>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="76"/>
-      <c r="AH4" s="76"/>
-      <c r="AI4" s="76"/>
-      <c r="AJ4" s="76"/>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="76"/>
-      <c r="AN4" s="76"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="76"/>
-      <c r="AT4" s="76"/>
+      <c r="A4" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
+      <c r="AE4" s="78"/>
+      <c r="AF4" s="78"/>
+      <c r="AG4" s="78"/>
+      <c r="AH4" s="78"/>
+      <c r="AI4" s="78"/>
+      <c r="AJ4" s="78"/>
+      <c r="AK4" s="78"/>
+      <c r="AL4" s="78"/>
+      <c r="AM4" s="78"/>
+      <c r="AN4" s="78"/>
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="78"/>
+      <c r="AT4" s="78"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
-      <c r="AB5" s="77"/>
-      <c r="AC5" s="77"/>
-      <c r="AD5" s="77"/>
-      <c r="AE5" s="77"/>
-      <c r="AF5" s="77"/>
-      <c r="AG5" s="77"/>
-      <c r="AH5" s="77"/>
-      <c r="AI5" s="77"/>
-      <c r="AJ5" s="77"/>
-      <c r="AK5" s="77"/>
-      <c r="AL5" s="77"/>
-      <c r="AM5" s="77"/>
-      <c r="AN5" s="77"/>
-      <c r="AO5" s="77"/>
-      <c r="AP5" s="77"/>
-      <c r="AQ5" s="77"/>
-      <c r="AR5" s="77"/>
-      <c r="AS5" s="77"/>
-      <c r="AT5" s="77"/>
+      <c r="A5" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="79"/>
+      <c r="AC5" s="79"/>
+      <c r="AD5" s="79"/>
+      <c r="AE5" s="79"/>
+      <c r="AF5" s="79"/>
+      <c r="AG5" s="79"/>
+      <c r="AH5" s="79"/>
+      <c r="AI5" s="79"/>
+      <c r="AJ5" s="79"/>
+      <c r="AK5" s="79"/>
+      <c r="AL5" s="79"/>
+      <c r="AM5" s="79"/>
+      <c r="AN5" s="79"/>
+      <c r="AO5" s="79"/>
+      <c r="AP5" s="79"/>
+      <c r="AQ5" s="79"/>
+      <c r="AR5" s="79"/>
+      <c r="AS5" s="79"/>
+      <c r="AT5" s="79"/>
       <c r="AU5" s="40"/>
     </row>
     <row r="6" s="40" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
-      <c r="AC6" s="78"/>
-      <c r="AD6" s="78"/>
-      <c r="AE6" s="78"/>
-      <c r="AF6" s="78"/>
-      <c r="AG6" s="78"/>
-      <c r="AH6" s="78"/>
-      <c r="AI6" s="78"/>
-      <c r="AJ6" s="78"/>
-      <c r="AK6" s="78"/>
-      <c r="AL6" s="78"/>
-      <c r="AM6" s="78"/>
-      <c r="AN6" s="78"/>
-      <c r="AO6" s="78"/>
-      <c r="AP6" s="78"/>
-      <c r="AQ6" s="78"/>
-      <c r="AR6" s="78"/>
-      <c r="AS6" s="78"/>
-      <c r="AT6" s="78"/>
+      <c r="A6" s="80" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="80"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="80"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="80"/>
+      <c r="Z6" s="80"/>
+      <c r="AA6" s="80"/>
+      <c r="AB6" s="80"/>
+      <c r="AC6" s="80"/>
+      <c r="AD6" s="80"/>
+      <c r="AE6" s="80"/>
+      <c r="AF6" s="80"/>
+      <c r="AG6" s="80"/>
+      <c r="AH6" s="80"/>
+      <c r="AI6" s="80"/>
+      <c r="AJ6" s="80"/>
+      <c r="AK6" s="80"/>
+      <c r="AL6" s="80"/>
+      <c r="AM6" s="80"/>
+      <c r="AN6" s="80"/>
+      <c r="AO6" s="80"/>
+      <c r="AP6" s="80"/>
+      <c r="AQ6" s="80"/>
+      <c r="AR6" s="80"/>
+      <c r="AS6" s="80"/>
+      <c r="AT6" s="80"/>
     </row>
     <row r="7" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
@@ -4868,7 +5138,7 @@
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
       <c r="E7" s="43" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
@@ -4914,15 +5184,15 @@
       <c r="M8" s="43"/>
       <c r="N8" s="43"/>
       <c r="O8" s="43"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="80"/>
-      <c r="S8" s="80"/>
-      <c r="T8" s="80"/>
-      <c r="U8" s="80"/>
-      <c r="V8" s="80"/>
-      <c r="W8" s="80"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="80"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="82"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="82"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="82"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="82"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44" t="s">
@@ -4942,16 +5212,16 @@
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="81" t="n">
+      <c r="H9" s="83" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="83"/>
       <c r="Q9" s="27" t="s">
         <v>6</v>
       </c>
@@ -4982,16 +5252,16 @@
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="81" t="n">
+      <c r="H10" s="83" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
       <c r="Q10" s="27" t="s">
         <v>9</v>
       </c>
@@ -5022,16 +5292,16 @@
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="82" t="n">
+      <c r="H11" s="84" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="84"/>
+      <c r="N11" s="84"/>
+      <c r="O11" s="84"/>
       <c r="Q11" s="27" t="s">
         <v>12</v>
       </c>
@@ -5045,154 +5315,164 @@
       <c r="Y11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="83" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
+      <c r="A12" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="87" t="n">
+        <v>4</v>
+      </c>
       <c r="D12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q12" s="87"/>
-      <c r="R12" s="87"/>
-      <c r="S12" s="87"/>
-      <c r="T12" s="87"/>
-      <c r="U12" s="87"/>
-      <c r="V12" s="87"/>
-      <c r="W12" s="87"/>
-      <c r="X12" s="87"/>
-      <c r="Y12" s="87"/>
-      <c r="Z12" s="87"/>
+      <c r="E12" s="88" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="89" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="90" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q12" s="90"/>
+      <c r="R12" s="90"/>
+      <c r="S12" s="90"/>
+      <c r="T12" s="90"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="90"/>
+      <c r="X12" s="90"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="90"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="84" t="s">
-        <v>100</v>
+      <c r="A13" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>120</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="88" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="87"/>
-      <c r="T13" s="87"/>
-      <c r="U13" s="87"/>
-      <c r="V13" s="87"/>
-      <c r="W13" s="87"/>
-      <c r="X13" s="87"/>
-      <c r="Y13" s="87"/>
-      <c r="Z13" s="87"/>
+      <c r="H13" s="91" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91"/>
+      <c r="O13" s="91"/>
+      <c r="P13" s="90" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q13" s="90"/>
+      <c r="R13" s="90"/>
+      <c r="S13" s="90"/>
+      <c r="T13" s="90"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="90"/>
+      <c r="W13" s="90"/>
+      <c r="X13" s="90"/>
+      <c r="Y13" s="90"/>
+      <c r="Z13" s="90"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="91" t="s">
+      <c r="A14" s="92" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="92" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="93" t="s">
-        <v>100</v>
-      </c>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="93"/>
-      <c r="N14" s="93"/>
-      <c r="O14" s="93"/>
-      <c r="P14" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="87"/>
-      <c r="S14" s="87"/>
-      <c r="T14" s="87"/>
-      <c r="U14" s="87"/>
-      <c r="V14" s="87"/>
-      <c r="W14" s="87"/>
-      <c r="X14" s="87"/>
-      <c r="Y14" s="87"/>
-      <c r="Z14" s="87"/>
+      <c r="E14" s="95" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="96" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="96"/>
+      <c r="P14" s="90" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="90"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="90"/>
+      <c r="X14" s="90"/>
+      <c r="Y14" s="90"/>
+      <c r="Z14" s="90"/>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="51" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="94"/>
-      <c r="O15" s="94"/>
-      <c r="P15" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="87"/>
-      <c r="T15" s="87"/>
-      <c r="U15" s="87"/>
-      <c r="V15" s="87"/>
-      <c r="W15" s="87"/>
-      <c r="X15" s="87"/>
-      <c r="Y15" s="87"/>
-      <c r="Z15" s="87"/>
+      <c r="E15" s="97" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="97"/>
+      <c r="O15" s="97"/>
+      <c r="P15" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q15" s="90"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="90"/>
+      <c r="T15" s="90"/>
+      <c r="U15" s="90"/>
+      <c r="V15" s="90"/>
+      <c r="W15" s="90"/>
+      <c r="X15" s="90"/>
+      <c r="Y15" s="90"/>
+      <c r="Z15" s="90"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
@@ -5219,7 +5499,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="53" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
@@ -5272,7 +5552,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="54" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B18" s="54"/>
       <c r="C18" s="54"/>
@@ -5328,245 +5608,245 @@
         <v>1</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D19" s="56" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G19" s="58"/>
       <c r="H19" s="57" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I19" s="58"/>
       <c r="J19" s="59" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="K19" s="58"/>
       <c r="L19" s="57" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="M19" s="58"/>
       <c r="N19" s="57" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="O19" s="58"/>
       <c r="P19" s="57" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="Q19" s="58"/>
       <c r="R19" s="57" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="S19" s="58"/>
       <c r="T19" s="57" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="U19" s="58"/>
       <c r="V19" s="57" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="W19" s="58"/>
       <c r="X19" s="59" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="Y19" s="58"/>
       <c r="Z19" s="57" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="AA19" s="58"/>
       <c r="AB19" s="57" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="AC19" s="58"/>
       <c r="AD19" s="57" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="AE19" s="58"/>
       <c r="AF19" s="57" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="AG19" s="58"/>
       <c r="AH19" s="57" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="AI19" s="58"/>
       <c r="AJ19" s="57" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="AK19" s="58"/>
       <c r="AL19" s="57" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="AM19" s="58"/>
       <c r="AN19" s="57" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="AO19" s="58"/>
       <c r="AP19" s="57" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="AQ19" s="58"/>
       <c r="AR19" s="57" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AS19" s="58"/>
       <c r="AT19" s="60" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AU19" s="60"/>
       <c r="AV19" s="60" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AW19" s="60"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="61"/>
       <c r="B20" s="62" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C20" s="62"/>
       <c r="D20" s="62"/>
       <c r="E20" s="62"/>
       <c r="F20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="I20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="J20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="K20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="L20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="M20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="N20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="O20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="P20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="Q20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="R20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="S20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="T20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="U20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="V20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="W20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="X20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="Y20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="Z20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AA20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AB20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AC20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AD20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AE20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AF20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AG20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AH20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AI20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AJ20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AK20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AL20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AM20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AN20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AO20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AP20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AQ20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AR20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AS20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AT20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AU20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="AV20" s="63" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="AW20" s="64" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5577,23 +5857,33 @@
         <v>4</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E21" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="67"/>
+        <v>92</v>
+      </c>
+      <c r="F21" s="67" t="s">
+        <v>46</v>
+      </c>
       <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
+      <c r="H21" s="67" t="s">
+        <v>93</v>
+      </c>
       <c r="I21" s="67"/>
-      <c r="J21" s="68"/>
+      <c r="J21" s="68" t="s">
+        <v>94</v>
+      </c>
       <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
+      <c r="L21" s="68" t="s">
+        <v>94</v>
+      </c>
       <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
+      <c r="N21" s="68" t="s">
+        <v>48</v>
+      </c>
       <c r="O21" s="68"/>
       <c r="P21" s="68"/>
       <c r="Q21" s="68"/>
@@ -5638,32 +5928,48 @@
         <v>7</v>
       </c>
       <c r="C22" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D22" s="71" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F22" s="73"/>
       <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
+      <c r="H22" s="73" t="s">
+        <v>97</v>
+      </c>
       <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
+      <c r="J22" s="73" t="s">
+        <v>93</v>
+      </c>
       <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
+      <c r="L22" s="73" t="s">
+        <v>98</v>
+      </c>
       <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
+      <c r="N22" s="73" t="s">
+        <v>98</v>
+      </c>
       <c r="O22" s="73"/>
-      <c r="P22" s="73"/>
+      <c r="P22" s="73" t="s">
+        <v>99</v>
+      </c>
       <c r="Q22" s="73"/>
-      <c r="R22" s="73"/>
-      <c r="S22" s="73"/>
-      <c r="T22" s="73"/>
-      <c r="U22" s="73"/>
-      <c r="V22" s="73"/>
-      <c r="W22" s="73"/>
+      <c r="R22" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="S22" s="74"/>
+      <c r="T22" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="U22" s="74"/>
+      <c r="V22" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="W22" s="74"/>
       <c r="X22" s="68"/>
       <c r="Y22" s="68"/>
       <c r="Z22" s="68"/>
@@ -5699,31 +6005,45 @@
         <v>10</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D23" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="74" t="s">
-        <v>87</v>
+        <v>100</v>
+      </c>
+      <c r="E23" s="75" t="s">
+        <v>101</v>
       </c>
       <c r="F23" s="73"/>
       <c r="G23" s="73"/>
       <c r="H23" s="73"/>
       <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
+      <c r="J23" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
+      <c r="L23" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
+      <c r="N23" s="73" t="s">
+        <v>102</v>
+      </c>
       <c r="O23" s="73"/>
-      <c r="P23" s="73"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
-      <c r="S23" s="73"/>
-      <c r="T23" s="73"/>
-      <c r="U23" s="73"/>
-      <c r="V23" s="73"/>
+      <c r="P23" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="U23" s="74"/>
+      <c r="V23" s="73" t="s">
+        <v>48</v>
+      </c>
       <c r="W23" s="73"/>
       <c r="X23" s="73"/>
       <c r="Y23" s="73"/>
@@ -5760,13 +6080,13 @@
         <v>10</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D24" s="70" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="F24" s="73"/>
       <c r="G24" s="73"/>
@@ -5774,24 +6094,38 @@
       <c r="I24" s="73"/>
       <c r="J24" s="73"/>
       <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
+      <c r="L24" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
+      <c r="N24" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="O24" s="73"/>
-      <c r="P24" s="73"/>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="73"/>
-      <c r="S24" s="73"/>
-      <c r="T24" s="73"/>
-      <c r="U24" s="73"/>
-      <c r="V24" s="73"/>
-      <c r="W24" s="73"/>
-      <c r="X24" s="68"/>
-      <c r="Y24" s="68"/>
-      <c r="Z24" s="68"/>
-      <c r="AA24" s="68"/>
-      <c r="AB24" s="68"/>
-      <c r="AC24" s="68"/>
+      <c r="P24" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="S24" s="76"/>
+      <c r="T24" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="U24" s="76"/>
+      <c r="V24" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="W24" s="76"/>
+      <c r="X24" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y24" s="76"/>
+      <c r="Z24" s="76"/>
+      <c r="AA24" s="76"/>
+      <c r="AB24" s="76"/>
+      <c r="AC24" s="76"/>
       <c r="AD24" s="68"/>
       <c r="AE24" s="68"/>
       <c r="AF24" s="68"/>
@@ -5821,13 +6155,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D25" s="70" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="F25" s="73"/>
       <c r="G25" s="73"/>
@@ -5837,23 +6171,41 @@
       <c r="K25" s="73"/>
       <c r="L25" s="73"/>
       <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
+      <c r="N25" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
+      <c r="P25" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="Q25" s="73"/>
-      <c r="R25" s="73"/>
-      <c r="S25" s="73"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="73"/>
-      <c r="V25" s="73"/>
-      <c r="W25" s="73"/>
-      <c r="X25" s="68"/>
-      <c r="Y25" s="68"/>
-      <c r="Z25" s="68"/>
-      <c r="AA25" s="68"/>
-      <c r="AB25" s="68"/>
-      <c r="AC25" s="68"/>
-      <c r="AD25" s="68"/>
+      <c r="R25" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="S25" s="74"/>
+      <c r="T25" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="W25" s="74"/>
+      <c r="X25" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y25" s="76"/>
+      <c r="Z25" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA25" s="76"/>
+      <c r="AB25" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC25" s="76"/>
+      <c r="AD25" s="68" t="s">
+        <v>48</v>
+      </c>
       <c r="AE25" s="68"/>
       <c r="AF25" s="68"/>
       <c r="AG25" s="68"/>
@@ -5882,13 +6234,13 @@
         <v>10</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D26" s="70" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="F26" s="68"/>
       <c r="G26" s="68"/>
@@ -5900,28 +6252,46 @@
       <c r="M26" s="68"/>
       <c r="N26" s="68"/>
       <c r="O26" s="68"/>
-      <c r="P26" s="73"/>
+      <c r="P26" s="73" t="s">
+        <v>46</v>
+      </c>
       <c r="Q26" s="73"/>
-      <c r="R26" s="73"/>
+      <c r="R26" s="73" t="s">
+        <v>1</v>
+      </c>
       <c r="S26" s="73"/>
-      <c r="T26" s="73"/>
+      <c r="T26" s="73" t="s">
+        <v>124</v>
+      </c>
       <c r="U26" s="73"/>
-      <c r="V26" s="73"/>
-      <c r="W26" s="73"/>
-      <c r="X26" s="73"/>
+      <c r="V26" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="W26" s="74"/>
+      <c r="X26" s="73" t="s">
+        <v>105</v>
+      </c>
       <c r="Y26" s="73"/>
-      <c r="Z26" s="73"/>
-      <c r="AA26" s="73"/>
-      <c r="AB26" s="73"/>
-      <c r="AC26" s="73"/>
-      <c r="AD26" s="73"/>
-      <c r="AE26" s="73"/>
-      <c r="AF26" s="68"/>
-      <c r="AG26" s="68"/>
-      <c r="AH26" s="73"/>
-      <c r="AI26" s="73"/>
-      <c r="AJ26" s="73"/>
-      <c r="AK26" s="73"/>
+      <c r="Z26" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA26" s="74"/>
+      <c r="AB26" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC26" s="74"/>
+      <c r="AD26" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE26" s="74"/>
+      <c r="AF26" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG26" s="76"/>
+      <c r="AH26" s="74"/>
+      <c r="AI26" s="74"/>
+      <c r="AJ26" s="74"/>
+      <c r="AK26" s="74"/>
       <c r="AL26" s="73"/>
       <c r="AM26" s="73"/>
       <c r="AN26" s="68"/>
@@ -5936,251 +6306,307 @@
       <c r="AW26" s="73"/>
     </row>
     <row r="27" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="95" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="95"/>
-      <c r="N27" s="95"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="95"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="95"/>
-      <c r="U27" s="95"/>
-      <c r="V27" s="95"/>
-      <c r="W27" s="95"/>
-      <c r="X27" s="95"/>
-      <c r="Y27" s="95"/>
-      <c r="Z27" s="95"/>
-      <c r="AA27" s="95"/>
-      <c r="AB27" s="95"/>
-      <c r="AC27" s="95"/>
-      <c r="AD27" s="95"/>
-      <c r="AE27" s="95"/>
-      <c r="AF27" s="95"/>
-      <c r="AG27" s="95"/>
-      <c r="AH27" s="95"/>
-      <c r="AI27" s="95"/>
-      <c r="AJ27" s="95"/>
-      <c r="AK27" s="95"/>
-      <c r="AL27" s="95"/>
-      <c r="AM27" s="95"/>
-      <c r="AN27" s="95"/>
-      <c r="AO27" s="95"/>
-      <c r="AP27" s="95"/>
-      <c r="AQ27" s="95"/>
-      <c r="AR27" s="95"/>
-      <c r="AS27" s="95"/>
-      <c r="AT27" s="95"/>
-      <c r="AU27" s="95"/>
-      <c r="AV27" s="95"/>
-      <c r="AW27" s="95"/>
+      <c r="A27" s="98" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="98"/>
+      <c r="N27" s="98"/>
+      <c r="O27" s="98"/>
+      <c r="P27" s="98"/>
+      <c r="Q27" s="98"/>
+      <c r="R27" s="98"/>
+      <c r="S27" s="98"/>
+      <c r="T27" s="98"/>
+      <c r="U27" s="98"/>
+      <c r="V27" s="98"/>
+      <c r="W27" s="98"/>
+      <c r="X27" s="98"/>
+      <c r="Y27" s="98"/>
+      <c r="Z27" s="98"/>
+      <c r="AA27" s="98"/>
+      <c r="AB27" s="98"/>
+      <c r="AC27" s="98"/>
+      <c r="AD27" s="98"/>
+      <c r="AE27" s="98"/>
+      <c r="AF27" s="98"/>
+      <c r="AG27" s="98"/>
+      <c r="AH27" s="98"/>
+      <c r="AI27" s="98"/>
+      <c r="AJ27" s="98"/>
+      <c r="AK27" s="98"/>
+      <c r="AL27" s="98"/>
+      <c r="AM27" s="98"/>
+      <c r="AN27" s="98"/>
+      <c r="AO27" s="98"/>
+      <c r="AP27" s="98"/>
+      <c r="AQ27" s="98"/>
+      <c r="AR27" s="98"/>
+      <c r="AS27" s="98"/>
+      <c r="AT27" s="98"/>
+      <c r="AU27" s="98"/>
+      <c r="AV27" s="98"/>
+      <c r="AW27" s="98"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="55"/>
-      <c r="B28" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="97" t="s">
-        <v>105</v>
+      <c r="B28" s="99" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="G28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="H28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="H28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="I28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="J28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="J28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="K28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="L28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="L28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="M28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="N28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="N28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="O28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="P28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="P28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="Q28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="R28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="R28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="S28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="T28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="T28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="U28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="V28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="V28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="W28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="X28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="X28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="Y28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="Z28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AA28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AB28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AC28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AD28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AE28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AF28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AG28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AH28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AI28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AJ28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AJ28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AK28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AL28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AL28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AM28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AN28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AN28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AO28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AP28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AQ28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AR28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AR28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AS28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AT28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AU28" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV28" s="97" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="AV28" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="AW28" s="64" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="55"/>
-      <c r="B29" s="96" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="98"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="98"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="98"/>
-      <c r="M29" s="99"/>
-      <c r="N29" s="98"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="98"/>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="98"/>
-      <c r="S29" s="99"/>
-      <c r="T29" s="98"/>
-      <c r="U29" s="99"/>
-      <c r="V29" s="98"/>
-      <c r="W29" s="99"/>
-      <c r="X29" s="98"/>
-      <c r="Y29" s="99"/>
-      <c r="Z29" s="98"/>
-      <c r="AA29" s="99"/>
-      <c r="AB29" s="98"/>
-      <c r="AC29" s="99"/>
-      <c r="AD29" s="98"/>
-      <c r="AE29" s="99"/>
-      <c r="AF29" s="98"/>
-      <c r="AG29" s="99"/>
-      <c r="AH29" s="98"/>
-      <c r="AI29" s="99"/>
-      <c r="AJ29" s="98"/>
-      <c r="AK29" s="99"/>
-      <c r="AL29" s="98"/>
-      <c r="AM29" s="99"/>
-      <c r="AN29" s="98"/>
-      <c r="AO29" s="99"/>
-      <c r="AP29" s="98"/>
-      <c r="AQ29" s="99"/>
-      <c r="AR29" s="98"/>
-      <c r="AS29" s="99"/>
-      <c r="AT29" s="98"/>
-      <c r="AU29" s="99"/>
-      <c r="AV29" s="98"/>
-      <c r="AW29" s="99"/>
+      <c r="B29" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="H29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="J29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="L29" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="M29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="N29" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="O29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="P29" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="R29" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="S29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="T29" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="U29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="V29" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="W29" s="102" t="n">
+        <v>5</v>
+      </c>
+      <c r="X29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF29" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="102" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH29" s="101"/>
+      <c r="AI29" s="102"/>
+      <c r="AJ29" s="101"/>
+      <c r="AK29" s="102"/>
+      <c r="AL29" s="101"/>
+      <c r="AM29" s="102"/>
+      <c r="AN29" s="101"/>
+      <c r="AO29" s="102"/>
+      <c r="AP29" s="101"/>
+      <c r="AQ29" s="102"/>
+      <c r="AR29" s="101"/>
+      <c r="AS29" s="102"/>
+      <c r="AT29" s="101"/>
+      <c r="AU29" s="102"/>
+      <c r="AV29" s="101"/>
+      <c r="AW29" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="176">

</xml_diff>